<commit_message>
Fix add SV and add About form
</commit_message>
<xml_diff>
--- a/QLSV/Student.xlsx
+++ b/QLSV/Student.xlsx
@@ -46,70 +46,70 @@
     <x:t>Rank</x:t>
   </x:si>
   <x:si>
-    <x:t>Lisa Green</x:t>
-  </x:si>
-  <x:si>
-    <x:t>321</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Female</x:t>
+    <x:t>Thảo Nhi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>456</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nữ</x:t>
   </x:si>
   <x:si>
     <x:t>Giỏi</x:t>
   </x:si>
   <x:si>
-    <x:t>Alex Chen</x:t>
-  </x:si>
-  <x:si>
-    <x:t>654</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Male</x:t>
+    <x:t>Văn B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>564</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Văn T</x:t>
+  </x:si>
+  <x:si>
+    <x:t>653</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trung Bình</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Văn Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>434</x:t>
+  </x:si>
+  <x:si>
+    <x:t>K</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5433</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Văn Kỳ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4354</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kém</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nhi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>213</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kiều Loan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>614</x:t>
   </x:si>
   <x:si>
     <x:t>Khá</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sarah Kim</x:t>
-  </x:si>
-  <x:si>
-    <x:t>987</x:t>
-  </x:si>
-  <x:si>
-    <x:t>David Lee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trung Bình</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Emily Wang</x:t>
-  </x:si>
-  <x:si>
-    <x:t>567</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kevin Liu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Olivia Tan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>543</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thảo Nhi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>456</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nữ</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -155,23 +155,16 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -474,7 +467,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J9"/>
+  <x:dimension ref="A1:J7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -526,19 +519,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E2" s="1">
-        <x:v>32957</x:v>
+        <x:v>37824.5513888889</x:v>
       </x:c>
       <x:c r="F2" s="0">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G2" s="0">
-        <x:v>8.7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H2" s="0">
-        <x:v>8.2</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I2" s="0">
-        <x:v>8.6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
         <x:v>13</x:v>
@@ -552,60 +545,60 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C3" s="0">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="E3" s="1">
-        <x:v>34523</x:v>
+        <x:v>38190.684537037</x:v>
       </x:c>
       <x:c r="F3" s="0">
-        <x:v>7.5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="G3" s="0">
-        <x:v>7.9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H3" s="0">
-        <x:v>6.5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="I3" s="0">
-        <x:v>7.3</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
       <x:c r="A4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="C4" s="0">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E4" s="1">
+        <x:v>37824.6858912037</x:v>
+      </x:c>
+      <x:c r="F4" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="G4" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H4" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I4" s="0">
+        <x:v>6.3</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="C4" s="0">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E4" s="1">
-        <x:v>33785</x:v>
-      </x:c>
-      <x:c r="F4" s="0">
-        <x:v>8.9</x:v>
-      </x:c>
-      <x:c r="G4" s="0">
-        <x:v>9.1</x:v>
-      </x:c>
-      <x:c r="H4" s="0">
-        <x:v>8.8</x:v>
-      </x:c>
-      <x:c r="I4" s="0">
-        <x:v>8.9</x:v>
-      </x:c>
-      <x:c r="J4" s="0" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:10">
@@ -622,86 +615,86 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="E5" s="1">
-        <x:v>33560</x:v>
+        <x:v>37824.6872337963</x:v>
       </x:c>
       <x:c r="F5" s="0">
-        <x:v>6.5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G5" s="0">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H5" s="0">
-        <x:v>7.2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="I5" s="0">
-        <x:v>6.9</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="C6" s="0">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E6" s="1">
+        <x:v>37824.688900463</x:v>
+      </x:c>
+      <x:c r="F6" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="G6" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H6" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="I6" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E6" s="1">
-        <x:v>34071</x:v>
-      </x:c>
-      <x:c r="F6" s="0">
-        <x:v>8.3</x:v>
-      </x:c>
-      <x:c r="G6" s="0">
-        <x:v>8.2</x:v>
-      </x:c>
-      <x:c r="H6" s="0">
-        <x:v>7.9</x:v>
-      </x:c>
-      <x:c r="I6" s="0">
-        <x:v>8.1</x:v>
-      </x:c>
-      <x:c r="J6" s="0" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10">
       <x:c r="A7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
       <x:c r="C7" s="0">
-        <x:v>21</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="E7" s="1">
-        <x:v>32744</x:v>
+        <x:v>39285.9286226852</x:v>
       </x:c>
       <x:c r="F7" s="0">
-        <x:v>7.6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G7" s="0">
-        <x:v>7.4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H7" s="0">
-        <x:v>7.8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="I7" s="0">
-        <x:v>7.6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10">
@@ -718,19 +711,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E8" s="1">
-        <x:v>33297</x:v>
+        <x:v>37824.9277083333</x:v>
       </x:c>
       <x:c r="F8" s="0">
-        <x:v>9.1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G8" s="0">
-        <x:v>9.2</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H8" s="0">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I8" s="0">
-        <x:v>9.1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="J8" s="0" t="s">
         <x:v>13</x:v>
@@ -744,28 +737,28 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C9" s="0">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E9" s="1">
+        <x:v>37459.9281365741</x:v>
+      </x:c>
+      <x:c r="F9" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="G9" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H9" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="I9" s="0">
+        <x:v>7.7</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="E9" s="2">
-        <x:v>37824.5517476852</x:v>
-      </x:c>
-      <x:c r="F9" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="G9" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="H9" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I9" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="J9" s="0" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Fix Update after update or change student's info and fix SortbyID
</commit_message>
<xml_diff>
--- a/QLSV/Student.xlsx
+++ b/QLSV/Student.xlsx
@@ -46,70 +46,76 @@
     <x:t>Rank</x:t>
   </x:si>
   <x:si>
-    <x:t>Thảo Nhi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>456</x:t>
+    <x:t>X</x:t>
+  </x:si>
+  <x:si>
+    <x:t>653</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trung Bình</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Văn Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>434</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kim</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5433</x:t>
   </x:si>
   <x:si>
     <x:t>Nữ</x:t>
   </x:si>
   <x:si>
+    <x:t>Khá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Văn Kỳ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4354</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kém</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trúc Lan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>213</x:t>
+  </x:si>
+  <x:si>
     <x:t>Giỏi</x:t>
   </x:si>
   <x:si>
-    <x:t>Văn B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>564</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nam</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Văn T</x:t>
-  </x:si>
-  <x:si>
-    <x:t>653</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trung Bình</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Văn Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>434</x:t>
-  </x:si>
-  <x:si>
-    <x:t>K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5433</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Văn Kỳ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4354</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kém</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nhi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>213</x:t>
-  </x:si>
-  <x:si>
     <x:t>Kiều Loan</x:t>
   </x:si>
   <x:si>
     <x:t>614</x:t>
   </x:si>
   <x:si>
-    <x:t>Khá</x:t>
+    <x:t>Thảo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>565</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Đỗ Tú</x:t>
+  </x:si>
+  <x:si>
+    <x:t>364</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bảo Ngọc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>854</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -467,7 +473,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J7"/>
+  <x:dimension ref="A1:J10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -519,19 +525,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E2" s="1">
-        <x:v>37824.5513888889</x:v>
+        <x:v>37825.0040046296</x:v>
       </x:c>
       <x:c r="F2" s="0">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G2" s="0">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="0">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="I2" s="0">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
         <x:v>13</x:v>
@@ -545,25 +551,25 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C3" s="0">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E3" s="1">
-        <x:v>38190.684537037</x:v>
+        <x:v>37824.6872337963</x:v>
       </x:c>
       <x:c r="F3" s="0">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G3" s="0">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H3" s="0">
-        <x:v>8</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="I3" s="0">
-        <x:v>8</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
         <x:v>13</x:v>
@@ -571,19 +577,19 @@
     </x:row>
     <x:row r="4" spans="1:10">
       <x:c r="A4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="C4" s="0">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C4" s="0">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="E4" s="1">
-        <x:v>37824.6858912037</x:v>
+        <x:v>38190.9721412037</x:v>
       </x:c>
       <x:c r="F4" s="0">
         <x:v>6</x:v>
@@ -592,10 +598,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H4" s="0">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I4" s="0">
-        <x:v>6.3</x:v>
+        <x:v>7.7</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
         <x:v>19</x:v>
@@ -609,100 +615,100 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C5" s="0">
-        <x:v>20</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E5" s="1">
-        <x:v>37824.6872337963</x:v>
+        <x:v>39285.9286226852</x:v>
       </x:c>
       <x:c r="F5" s="0">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G5" s="0">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H5" s="0">
-        <x:v>5</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="I5" s="0">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C6" s="0">
-        <x:v>20</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E6" s="1">
-        <x:v>37824.688900463</x:v>
+        <x:v>35633.9890625</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G6" s="0">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="H6" s="0">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I6" s="0">
-        <x:v>5</x:v>
+        <x:v>8.3</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10">
       <x:c r="A7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C7" s="0">
-        <x:v>16</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E7" s="1">
-        <x:v>39285.9286226852</x:v>
+        <x:v>37459.9281365741</x:v>
       </x:c>
       <x:c r="F7" s="0">
         <x:v>7</x:v>
       </x:c>
       <x:c r="G7" s="0">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H7" s="0">
-        <x:v>2</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I7" s="0">
-        <x:v>4</x:v>
+        <x:v>7.7</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10">
       <x:c r="A8" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C8" s="0">
         <x:v>20</x:v>
@@ -711,19 +717,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E8" s="1">
-        <x:v>37824.9277083333</x:v>
+        <x:v>37824.9739467593</x:v>
       </x:c>
       <x:c r="F8" s="0">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G8" s="0">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H8" s="0">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I8" s="0">
-        <x:v>10</x:v>
+        <x:v>6.3</x:v>
       </x:c>
       <x:c r="J8" s="0" t="s">
         <x:v>13</x:v>
@@ -731,34 +737,66 @@
     </x:row>
     <x:row r="9" spans="1:10">
       <x:c r="A9" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C9" s="0">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E9" s="1">
-        <x:v>37459.9281365741</x:v>
+        <x:v>35998.9777546296</x:v>
       </x:c>
       <x:c r="F9" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="G9" s="0">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="G9" s="0">
+      <x:c r="H9" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I9" s="0">
+        <x:v>6.7</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="A10" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C10" s="0">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E10" s="1">
+        <x:v>36363.9772569444</x:v>
+      </x:c>
+      <x:c r="F10" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G10" s="0">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H9" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I9" s="0">
-        <x:v>7.7</x:v>
-      </x:c>
-      <x:c r="J9" s="0" t="s">
-        <x:v>31</x:v>
+      <x:c r="H10" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="I10" s="0">
+        <x:v>4.3</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>